<commit_message>
Fixed linking + IDs
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0E9236-7E2C-466E-B72C-743D8F37DE40}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176F1171-EB1C-4DDE-BD98-F2AC1D684366}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="131">
   <si>
     <t>setting_name</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>end screen</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>REGDIA</t>
@@ -332,12 +329,6 @@
     <t>ID da criança</t>
   </si>
   <si>
-    <t>linked_table</t>
-  </si>
-  <si>
-    <t>{}</t>
-  </si>
-  <si>
     <t>string</t>
   </si>
   <si>
@@ -383,24 +374,9 @@
     <t>Type?</t>
   </si>
   <si>
-    <t>REGIDC = ?</t>
-  </si>
-  <si>
-    <t>[data('REGIDC')]</t>
-  </si>
-  <si>
-    <t>{REGIDC: data('REGIDC')}</t>
-  </si>
-  <si>
-    <t>CRIANCA_VISIT</t>
-  </si>
-  <si>
     <t>CRIANCA</t>
   </si>
   <si>
-    <t>visit</t>
-  </si>
-  <si>
     <t>Children</t>
   </si>
   <si>
@@ -456,6 +432,9 @@
   </si>
   <si>
     <t>LASTVISIT</t>
+  </si>
+  <si>
+    <t>REGID</t>
   </si>
 </sst>
 </file>
@@ -557,7 +536,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -577,7 +556,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -907,7 +885,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -923,7 +901,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -931,10 +909,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,7 +965,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1043,16 +1021,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F3" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>77</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1060,16 +1038,16 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
         <v>80</v>
       </c>
-      <c r="F4" t="s">
-        <v>81</v>
-      </c>
       <c r="G4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H4" t="s">
         <v>88</v>
-      </c>
-      <c r="H4" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1080,10 +1058,10 @@
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1098,39 +1076,39 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>54</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>55</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>56</v>
-      </c>
-      <c r="H8" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E9" t="s">
+        <v>57</v>
+      </c>
+      <c r="F9" t="s">
         <v>58</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>60</v>
-      </c>
-      <c r="H9" t="s">
-        <v>60</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -1138,13 +1116,13 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
+        <v>61</v>
+      </c>
+      <c r="G10" t="s">
         <v>62</v>
       </c>
-      <c r="G10" t="s">
-        <v>63</v>
-      </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J10" s="13"/>
     </row>
@@ -1163,13 +1141,13 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="G13" t="s">
-        <v>71</v>
-      </c>
       <c r="H13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -1177,13 +1155,13 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" t="s">
         <v>72</v>
       </c>
-      <c r="G14" t="s">
-        <v>73</v>
-      </c>
       <c r="H14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -1191,13 +1169,13 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" t="s">
         <v>74</v>
       </c>
-      <c r="G15" t="s">
-        <v>75</v>
-      </c>
       <c r="H15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -1215,13 +1193,13 @@
         <v>25</v>
       </c>
       <c r="F18" t="s">
+        <v>92</v>
+      </c>
+      <c r="G18" t="s">
         <v>93</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>94</v>
-      </c>
-      <c r="H18" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1239,43 +1217,43 @@
         <v>22</v>
       </c>
       <c r="E21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F23" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
@@ -1292,18 +1270,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="38" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
@@ -1340,78 +1319,52 @@
         <v>41</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
       <c r="H2" s="10"/>
       <c r="J2" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
       <c r="J3" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>118</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
-      </c>
-      <c r="C5" t="s">
-        <v>116</v>
-      </c>
-      <c r="D5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F5" t="s">
-        <v>114</v>
-      </c>
-      <c r="G5" t="s">
-        <v>115</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K6" s="14"/>
+      <c r="K5" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1454,13 +1407,13 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,92 +1458,92 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B5" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" t="s">
         <v>82</v>
-      </c>
-      <c r="D5" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1605,7 +1558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="A1:C1048576"/>
+      <selection pane="bottomLeft" sqref="A1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,10 +1581,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1639,7 +1592,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1650,10 +1603,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1661,10 +1614,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1672,7 +1625,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -1683,7 +1636,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -1694,7 +1647,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1705,7 +1658,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1716,7 +1669,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" t="s">
         <v>25</v>
@@ -1727,7 +1680,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>50</v>
+        <v>130</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -1749,7 +1702,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
@@ -1760,7 +1713,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>32</v>
@@ -1771,10 +1724,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1782,10 +1735,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>124</v>
+        <v>115</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1793,10 +1746,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1804,10 +1757,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1815,10 +1768,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>124</v>
+        <v>119</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1826,10 +1779,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -1837,10 +1790,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1848,10 +1801,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>124</v>
+        <v>122</v>
+      </c>
+      <c r="B24" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1859,10 +1812,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -1870,10 +1823,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1881,10 +1834,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>133</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1892,10 +1845,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1903,21 +1856,21 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>124</v>
+      <c r="A30" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B30" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed: ID (once again)
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176F1171-EB1C-4DDE-BD98-F2AC1D684366}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C8B953-2955-43EB-8F1C-7503C503ACBD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1558,7 +1558,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:C1048576"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1672,7 +1672,7 @@
         <v>92</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1683,7 +1683,7 @@
         <v>130</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -1705,7 +1705,7 @@
         <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Changed date format, and mad changes in CRIANCA_VISIT
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7A0A2B6-2DB4-4C74-A5AE-7DB348D2B975}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA5B27A-3DDB-4535-B456-1F9E61ADC544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="135">
   <si>
     <t>setting_name</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t xml:space="preserve">text </t>
+  </si>
+  <si>
+    <t>adate</t>
+  </si>
+  <si>
+    <t>Save only mm.dd.yyyy with support for ?? at all positions</t>
   </si>
 </sst>
 </file>
@@ -542,7 +548,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -557,7 +563,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -969,9 +974,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1058,7 +1063,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="F5" t="s">
         <v>42</v>
@@ -1113,7 +1118,7 @@
       <c r="H9" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="13" t="s">
+      <c r="J9" s="12" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1130,7 +1135,7 @@
       <c r="H10" t="s">
         <v>62</v>
       </c>
-      <c r="J10" s="13"/>
+      <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
@@ -1196,7 +1201,7 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>25</v>
+        <v>75</v>
       </c>
       <c r="F18" t="s">
         <v>92</v>
@@ -1370,7 +1375,7 @@
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K5" s="14"/>
+      <c r="K5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1383,7 +1388,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:D2"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1423,8 +1428,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="9"/>
+      <c r="A3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1562,9 +1577,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1700,7 +1715,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1722,7 +1737,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>32</v>
+        <v>133</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1743,7 +1758,7 @@
       <c r="A18" t="s">
         <v>115</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C18" t="b">
@@ -1776,7 +1791,7 @@
       <c r="A21" t="s">
         <v>119</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C21" t="b">
@@ -1809,7 +1824,7 @@
       <c r="A24" t="s">
         <v>122</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C24" t="b">
@@ -1842,7 +1857,7 @@
       <c r="A27" t="s">
         <v>125</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C27" t="b">
@@ -1872,10 +1887,10 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="16" t="s">
+      <c r="A30" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>116</v>
       </c>
       <c r="C30" t="b">

</xml_diff>

<commit_message>
New Surveys + minor fixes
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA5B27A-3DDB-4535-B456-1F9E61ADC544}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE253E-8B89-4498-B748-64E86F649C6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
   <si>
     <t>setting_name</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>Save only mm.dd.yyyy with support for ?? at all positions</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
   </si>
 </sst>
 </file>
@@ -972,11 +975,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,9 +994,10 @@
     <col min="8" max="8" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -1024,13 +1028,16 @@
       <c r="J1" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>75</v>
       </c>
@@ -1044,7 +1051,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>22</v>
       </c>
@@ -1061,7 +1068,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
         <v>133</v>
       </c>
@@ -1075,17 +1082,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>52</v>
       </c>
@@ -1102,7 +1109,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
         <v>52</v>
       </c>
@@ -1118,11 +1125,11 @@
       <c r="H9" t="s">
         <v>59</v>
       </c>
-      <c r="J9" s="12" t="s">
+      <c r="K9" s="12" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>25</v>
       </c>
@@ -1137,17 +1144,17 @@
       </c>
       <c r="J10" s="12"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>25</v>
       </c>
@@ -1161,7 +1168,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>25</v>
       </c>
@@ -1175,7 +1182,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>25</v>
       </c>
@@ -1189,7 +1196,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
Fixed linked tables icluding new hosp. and fal.
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DDE253E-8B89-4498-B748-64E86F649C6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23615F4-4DB5-4408-A934-609FFAC4F1B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -407,15 +407,6 @@
     <t>IDCOMSUP</t>
   </si>
   <si>
-    <t>PARMA</t>
-  </si>
-  <si>
-    <t>DAPARMA</t>
-  </si>
-  <si>
-    <t>IDPARMA</t>
-  </si>
-  <si>
     <t>MOMA</t>
   </si>
   <si>
@@ -450,6 +441,15 @@
   </si>
   <si>
     <t>choice_filter</t>
+  </si>
+  <si>
+    <t>PAMA</t>
+  </si>
+  <si>
+    <t>IDPAMA</t>
+  </si>
+  <si>
+    <t>DAPAMA</t>
   </si>
 </sst>
 </file>
@@ -977,9 +977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H12" sqref="H12"/>
+      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,7 +1029,7 @@
         <v>31</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F5" t="s">
         <v>42</v>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
         <v>95</v>
@@ -1445,7 +1445,7 @@
         <v>95</v>
       </c>
       <c r="D3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1584,9 +1584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1708,7 +1708,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B12" t="s">
         <v>75</v>
@@ -1722,7 +1722,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1744,7 +1744,7 @@
         <v>50</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B23" s="11" t="s">
         <v>114</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B24" s="14" t="s">
         <v>116</v>
@@ -1840,7 +1840,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B25" s="11" t="s">
         <v>114</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>114</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>116</v>
@@ -1873,7 +1873,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>114</v>
@@ -1884,10 +1884,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B29" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1895,7 +1895,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B30" s="14" t="s">
         <v>116</v>
@@ -1906,10 +1906,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B32" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Link from pregnancy to new child
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23615F4-4DB5-4408-A934-609FFAC4F1B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6F1E56-3C26-4CEB-A6FA-B6C72A403592}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="135">
   <si>
     <t>setting_name</t>
   </si>
@@ -172,9 +172,6 @@
   </si>
   <si>
     <t>english</t>
-  </si>
-  <si>
-    <t>GRAVIDA_ESTADO</t>
   </si>
   <si>
     <t>begin screen</t>
@@ -859,9 +856,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -899,7 +896,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -923,10 +920,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
         <v>111</v>
-      </c>
-      <c r="D5" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -964,7 +961,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1029,26 +1026,26 @@
         <v>31</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
         <v>75</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>76</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>77</v>
-      </c>
-      <c r="H3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1056,77 +1053,77 @@
         <v>22</v>
       </c>
       <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s">
         <v>79</v>
       </c>
-      <c r="F4" t="s">
-        <v>80</v>
-      </c>
       <c r="G4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" t="s">
         <v>87</v>
-      </c>
-      <c r="H4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F5" t="s">
         <v>42</v>
       </c>
       <c r="G5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="F8" t="s">
         <v>53</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>55</v>
-      </c>
-      <c r="H8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
         <v>57</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>58</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="12" t="s">
         <v>59</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -1134,24 +1131,24 @@
         <v>25</v>
       </c>
       <c r="F10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G10" t="s">
         <v>61</v>
       </c>
-      <c r="G10" t="s">
-        <v>62</v>
-      </c>
       <c r="H10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -1159,13 +1156,13 @@
         <v>25</v>
       </c>
       <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G13" t="s">
         <v>69</v>
       </c>
-      <c r="G13" t="s">
-        <v>70</v>
-      </c>
       <c r="H13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -1173,13 +1170,13 @@
         <v>25</v>
       </c>
       <c r="F14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" t="s">
         <v>71</v>
       </c>
-      <c r="G14" t="s">
-        <v>72</v>
-      </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1187,47 +1184,47 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
         <v>73</v>
       </c>
-      <c r="G15" t="s">
-        <v>74</v>
-      </c>
       <c r="H15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" t="s">
         <v>92</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>93</v>
-      </c>
-      <c r="H18" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
@@ -1235,48 +1232,48 @@
         <v>22</v>
       </c>
       <c r="E21" t="s">
+        <v>97</v>
+      </c>
+      <c r="F21" t="s">
         <v>98</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>100</v>
-      </c>
       <c r="H21" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C22" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1337,45 +1334,45 @@
         <v>41</v>
       </c>
       <c r="J1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
       <c r="H2" s="10"/>
       <c r="J2" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>66</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
       <c r="J3" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1425,27 +1422,27 @@
         <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
         <v>95</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>96</v>
-      </c>
-      <c r="D2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" t="s">
         <v>130</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1486,92 +1483,92 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D2" t="s">
         <v>101</v>
-      </c>
-      <c r="D2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D3" t="s">
         <v>103</v>
-      </c>
-      <c r="D3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" t="s">
         <v>81</v>
-      </c>
-      <c r="D5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1584,7 +1581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
@@ -1609,10 +1606,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1620,7 +1617,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1631,10 +1628,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1642,10 +1639,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1653,7 +1650,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -1664,7 +1661,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -1675,7 +1672,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1686,7 +1683,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1697,10 +1694,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
@@ -1708,10 +1705,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C12" t="b">
         <v>0</v>
@@ -1722,7 +1719,7 @@
         <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1730,10 +1727,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1741,10 +1738,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
@@ -1752,10 +1749,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>112</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="C17" t="b">
         <v>0</v>
@@ -1763,10 +1760,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>114</v>
+      </c>
+      <c r="B18" s="14" t="s">
         <v>115</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>116</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1774,10 +1771,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1785,10 +1782,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1796,10 +1793,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1807,10 +1804,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -1818,10 +1815,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1829,10 +1826,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1840,10 +1837,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -1851,10 +1848,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1862,10 +1859,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1873,10 +1870,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1884,10 +1881,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>123</v>
+      </c>
+      <c r="B29" t="s">
         <v>124</v>
-      </c>
-      <c r="B29" t="s">
-        <v>125</v>
       </c>
       <c r="C29" t="b">
         <v>0</v>
@@ -1895,10 +1892,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C30" t="b">
         <v>0</v>
@@ -1906,10 +1903,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B32" t="s">
         <v>128</v>
-      </c>
-      <c r="B32" t="s">
-        <v>129</v>
       </c>
       <c r="C32" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Fixed "NS" in questions + etn and inf in MIF
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6F1E56-3C26-4CEB-A6FA-B6C72A403592}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182EBEBE-59FB-4663-9202-FD07A8A3F321}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -856,7 +856,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
@@ -974,7 +974,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
     </sheetView>

</xml_diff>

<commit_message>
Added vatiables from "Depois do parto" to child
</commit_message>
<xml_diff>
--- a/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
+++ b/app/config/tables/CRIANCA/forms/CRIANCA/CRIANCA.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{182EBEBE-59FB-4663-9202-FD07A8A3F321}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92863A60-78BB-4612-84D6-C815F0A829E8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-2100" windowWidth="19440" windowHeight="15000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="settings" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="264">
   <si>
     <t>setting_name</t>
   </si>
@@ -129,9 +129,6 @@
     <t>comment</t>
   </si>
   <si>
-    <t>custom_date</t>
-  </si>
-  <si>
     <t>query_name</t>
   </si>
   <si>
@@ -196,9 +193,6 @@
   </si>
   <si>
     <t>Region</t>
-  </si>
-  <si>
-    <t>Região</t>
   </si>
   <si>
     <t>tabanca_csv</t>
@@ -329,12 +323,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>Makes the date widget DD/MM/YYYY</t>
-  </si>
-  <si>
     <t>YesNoU</t>
   </si>
   <si>
@@ -447,6 +435,405 @@
   </si>
   <si>
     <t>DAPAMA</t>
+  </si>
+  <si>
+    <t>assign</t>
+  </si>
+  <si>
+    <t>Região: {{data.regmif}}</t>
+  </si>
+  <si>
+    <t>Tabanca: {{data.tabmif}}</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>inf1</t>
+  </si>
+  <si>
+    <t>Informant</t>
+  </si>
+  <si>
+    <t>Informador</t>
+  </si>
+  <si>
+    <t>data('inf1') == '2'</t>
+  </si>
+  <si>
+    <t>inf2</t>
+  </si>
+  <si>
+    <t>Other informant</t>
+  </si>
+  <si>
+    <t>Outro informador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end if </t>
+  </si>
+  <si>
+    <t>GRINFOS</t>
+  </si>
+  <si>
+    <t>data('inf2')</t>
+  </si>
+  <si>
+    <t>data('inf1')</t>
+  </si>
+  <si>
+    <t>GRCONS</t>
+  </si>
+  <si>
+    <t>Did the woman seek consultations during pregnancy?</t>
+  </si>
+  <si>
+    <t>vpcard</t>
+  </si>
+  <si>
+    <t>CART_ANC</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>GRVAC</t>
+  </si>
+  <si>
+    <t>Vacina anti-tetánica durante esta gravidez?</t>
+  </si>
+  <si>
+    <t>data('GRVAC') == '1'</t>
+  </si>
+  <si>
+    <t>VACTTHI</t>
+  </si>
+  <si>
+    <t>vac. Hist</t>
+  </si>
+  <si>
+    <t>note</t>
+  </si>
+  <si>
+    <t>How many prenatal consultations?</t>
+  </si>
+  <si>
+    <t>Quantas consultas pré-natais durante esta gravidez?</t>
+  </si>
+  <si>
+    <t>CDG_M</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>Mulher</t>
+  </si>
+  <si>
+    <t>data('CART_ANC') == 'VIC'</t>
+  </si>
+  <si>
+    <t>CDG_C</t>
+  </si>
+  <si>
+    <t>Cartão</t>
+  </si>
+  <si>
+    <t>Number of times received iron/FA</t>
+  </si>
+  <si>
+    <t>A grávida recebeu comprimidos com ferro quantas vezes?</t>
+  </si>
+  <si>
+    <t>FEDEP_M</t>
+  </si>
+  <si>
+    <t>FEDEP_C</t>
+  </si>
+  <si>
+    <t>A grávida recebeu fansidar (TPI, SP) quantas vezes?</t>
+  </si>
+  <si>
+    <t>QVFANSI_M</t>
+  </si>
+  <si>
+    <t>QVFANSI_C</t>
+  </si>
+  <si>
+    <t>TABPART</t>
+  </si>
+  <si>
+    <t>Did the woman give birth in the village?</t>
+  </si>
+  <si>
+    <t>facility</t>
+  </si>
+  <si>
+    <t>LOCPAR</t>
+  </si>
+  <si>
+    <t>Where did the woman give birth?</t>
+  </si>
+  <si>
+    <t>healthstaff</t>
+  </si>
+  <si>
+    <t>ASSISTPART</t>
+  </si>
+  <si>
+    <t>Who assisted the birth?</t>
+  </si>
+  <si>
+    <t>data('PREGID') == null</t>
+  </si>
+  <si>
+    <t>LITTERSIZE</t>
+  </si>
+  <si>
+    <t>Number of children born</t>
+  </si>
+  <si>
+    <t>Self</t>
+  </si>
+  <si>
+    <t>Ela/e</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Outra/o</t>
+  </si>
+  <si>
+    <t>Mother</t>
+  </si>
+  <si>
+    <t>Mãe</t>
+  </si>
+  <si>
+    <t>Father</t>
+  </si>
+  <si>
+    <t>Pai</t>
+  </si>
+  <si>
+    <t>Mothers mother</t>
+  </si>
+  <si>
+    <t>Avó</t>
+  </si>
+  <si>
+    <t>Other family member</t>
+  </si>
+  <si>
+    <t>Outra mebro da familia</t>
+  </si>
+  <si>
+    <t>No informant found</t>
+  </si>
+  <si>
+    <t>Nenhum informador</t>
+  </si>
+  <si>
+    <t>Not applicable</t>
+  </si>
+  <si>
+    <t>Não aplicável</t>
+  </si>
+  <si>
+    <t>Missing</t>
+  </si>
+  <si>
+    <t>Falta informacao</t>
+  </si>
+  <si>
+    <t>HO</t>
+  </si>
+  <si>
+    <t>Hospital</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>Health Center</t>
+  </si>
+  <si>
+    <t>Centro de Saude</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Health Unit</t>
+  </si>
+  <si>
+    <t>Unidade de Saude Base</t>
+  </si>
+  <si>
+    <t>CA</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>OU</t>
+  </si>
+  <si>
+    <t>Elsewhere</t>
+  </si>
+  <si>
+    <t>Outro</t>
+  </si>
+  <si>
+    <t>DR</t>
+  </si>
+  <si>
+    <t>Doctor</t>
+  </si>
+  <si>
+    <t>Medico</t>
+  </si>
+  <si>
+    <t>PA</t>
+  </si>
+  <si>
+    <t>Midwife</t>
+  </si>
+  <si>
+    <t>Parteira</t>
+  </si>
+  <si>
+    <t>EN</t>
+  </si>
+  <si>
+    <t>Nurse</t>
+  </si>
+  <si>
+    <t>Enfermeira/o</t>
+  </si>
+  <si>
+    <t>MA-N</t>
+  </si>
+  <si>
+    <t>Traditional birth attendant - no course</t>
+  </si>
+  <si>
+    <t>Matrona - sem curso</t>
+  </si>
+  <si>
+    <t>MA-F</t>
+  </si>
+  <si>
+    <t>Traditional birth attendant - course</t>
+  </si>
+  <si>
+    <t>Matrona - formado</t>
+  </si>
+  <si>
+    <t>FA</t>
+  </si>
+  <si>
+    <t>Family member</t>
+  </si>
+  <si>
+    <t>Familia</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>Neighbour</t>
+  </si>
+  <si>
+    <t>Vizinho</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>No one</t>
+  </si>
+  <si>
+    <t>Ninguem</t>
+  </si>
+  <si>
+    <t>VIC</t>
+  </si>
+  <si>
+    <t>Card seen</t>
+  </si>
+  <si>
+    <t>Cartão visto</t>
+  </si>
+  <si>
+    <t>NTN</t>
+  </si>
+  <si>
+    <t>Has no card and no ANC</t>
+  </si>
+  <si>
+    <t>Não tem cartão e não tem consultas</t>
+  </si>
+  <si>
+    <t>NTS</t>
+  </si>
+  <si>
+    <t>Has no card, some ANC</t>
+  </si>
+  <si>
+    <t>Não tem cartão, mas tem consultas</t>
+  </si>
+  <si>
+    <t>NVC</t>
+  </si>
+  <si>
+    <t>Not brought card</t>
+  </si>
+  <si>
+    <t>Não trouxe o cartão</t>
+  </si>
+  <si>
+    <t>PC</t>
+  </si>
+  <si>
+    <t>Lost card</t>
+  </si>
+  <si>
+    <t>Perdeu o cartão</t>
+  </si>
+  <si>
+    <t>VCN</t>
+  </si>
+  <si>
+    <t>Card seen and ANCs</t>
+  </si>
+  <si>
+    <t>Cartão visto, mas sem consultas registadas</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>data('PREGID') != null</t>
+  </si>
+  <si>
+    <t>birthstatus</t>
+  </si>
+  <si>
+    <t>NADOESTADO</t>
+  </si>
+  <si>
+    <t>Status of child</t>
+  </si>
+  <si>
+    <t>Died before birth</t>
+  </si>
+  <si>
+    <t>Died after birth</t>
+  </si>
+  <si>
+    <t>Alive</t>
   </si>
 </sst>
 </file>
@@ -456,7 +843,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-406]General"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,15 +889,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -520,6 +900,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,7 +934,7 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -564,13 +950,15 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="2" xr:uid="{C28CC074-D3A0-48A2-81F3-B6A5CA836B7C}"/>
@@ -879,13 +1267,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>16</v>
@@ -896,7 +1284,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -912,7 +1300,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -920,10 +1308,10 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D5" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,7 +1327,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -961,7 +1349,7 @@
         <v>28</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -972,11 +1360,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F97EDFF-72E2-4781-A226-FCA8C7C63015}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1014,7 +1402,7 @@
         <v>10</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>11</v>
@@ -1026,157 +1414,154 @@
         <v>31</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="16"/>
+    </row>
+    <row r="4" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="D4" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>260</v>
+      </c>
+      <c r="I4" s="16"/>
+    </row>
+    <row r="5" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
-        <v>76</v>
-      </c>
-      <c r="H3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" t="s">
-        <v>79</v>
-      </c>
-      <c r="G4" t="s">
-        <v>86</v>
-      </c>
-      <c r="H4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" t="s">
-        <v>89</v>
-      </c>
-      <c r="H5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="B6" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>52</v>
+        <v>72</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="H8" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D9" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>76</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="H9" t="s">
-        <v>58</v>
-      </c>
-      <c r="K9" s="12" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="F10" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="G10" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="H10" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="12"/>
+        <v>86</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="H13" t="s">
-        <v>69</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>25</v>
+        <v>50</v>
+      </c>
+      <c r="E14" t="s">
+        <v>54</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="G14" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>133</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -1184,96 +1569,656 @@
         <v>25</v>
       </c>
       <c r="F15" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G15" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>73</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="J15" s="12"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="H19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" t="s">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F23" t="s">
+        <v>89</v>
+      </c>
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
+      <c r="H23" t="s">
         <v>91</v>
       </c>
-      <c r="G18" t="s">
-        <v>92</v>
-      </c>
-      <c r="H18" t="s">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="F26" t="s">
+        <v>94</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" t="s">
+        <v>102</v>
+      </c>
+      <c r="G28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="15"/>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>22</v>
       </c>
-      <c r="E21" t="s">
-        <v>97</v>
-      </c>
-      <c r="F21" t="s">
-        <v>98</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C22" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>74</v>
-      </c>
-      <c r="F23" t="s">
-        <v>106</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>48</v>
+      <c r="E33" t="s">
+        <v>135</v>
+      </c>
+      <c r="F33" t="s">
+        <v>135</v>
+      </c>
+      <c r="G33" t="s">
+        <v>136</v>
+      </c>
+      <c r="H33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G35" t="s">
+        <v>140</v>
+      </c>
+      <c r="H35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" t="s">
+        <v>143</v>
+      </c>
+      <c r="I38" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>131</v>
+      </c>
+      <c r="F40" t="s">
+        <v>143</v>
+      </c>
+      <c r="I40" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>25</v>
+      </c>
+      <c r="F44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
+        <v>22</v>
+      </c>
+      <c r="E47" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" t="s">
+        <v>146</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D50" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" t="s">
+        <v>148</v>
+      </c>
+      <c r="F50" t="s">
+        <v>149</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="H50" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D53" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" t="s">
+        <v>151</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+      <c r="C54" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D55" t="s">
+        <v>25</v>
+      </c>
+      <c r="F55" t="s">
+        <v>154</v>
+      </c>
+      <c r="G55" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>156</v>
+      </c>
+      <c r="G59" t="s">
+        <v>157</v>
+      </c>
+      <c r="H59" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D60" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" t="s">
+        <v>159</v>
+      </c>
+      <c r="G60" t="s">
+        <v>160</v>
+      </c>
+      <c r="H60" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+      <c r="C61" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D62" t="s">
+        <v>25</v>
+      </c>
+      <c r="F62" t="s">
+        <v>163</v>
+      </c>
+      <c r="G62" t="s">
+        <v>150</v>
+      </c>
+      <c r="H62" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D66" t="s">
+        <v>156</v>
+      </c>
+      <c r="G66" t="s">
+        <v>165</v>
+      </c>
+      <c r="H66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D67" t="s">
+        <v>25</v>
+      </c>
+      <c r="F67" t="s">
+        <v>167</v>
+      </c>
+      <c r="G67" t="s">
+        <v>160</v>
+      </c>
+      <c r="H67" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+      <c r="C68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D69" t="s">
+        <v>25</v>
+      </c>
+      <c r="F69" t="s">
+        <v>168</v>
+      </c>
+      <c r="G69" t="s">
+        <v>150</v>
+      </c>
+      <c r="H69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D73" t="s">
+        <v>156</v>
+      </c>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D74" t="s">
+        <v>25</v>
+      </c>
+      <c r="F74" t="s">
+        <v>170</v>
+      </c>
+      <c r="G74" t="s">
+        <v>160</v>
+      </c>
+      <c r="H74" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+      <c r="C75" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D76" t="s">
+        <v>25</v>
+      </c>
+      <c r="F76" t="s">
+        <v>171</v>
+      </c>
+      <c r="G76" t="s">
+        <v>150</v>
+      </c>
+      <c r="H76" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="D80" t="s">
+        <v>22</v>
+      </c>
+      <c r="E80" t="s">
+        <v>93</v>
+      </c>
+      <c r="F80" t="s">
+        <v>172</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D83" t="s">
+        <v>22</v>
+      </c>
+      <c r="E83" t="s">
+        <v>174</v>
+      </c>
+      <c r="F83" t="s">
+        <v>175</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="H83" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D86" t="s">
+        <v>22</v>
+      </c>
+      <c r="E86" t="s">
+        <v>177</v>
+      </c>
+      <c r="F86" t="s">
+        <v>178</v>
+      </c>
+      <c r="G86" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="15"/>
+      <c r="B88" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1285,7 +2230,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB23FD29-3338-4879-B1BD-848935333D8A}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1307,79 +2252,76 @@
   <sheetData>
     <row r="1" spans="1:11" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="E1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="7" t="s">
-        <v>41</v>
-      </c>
       <c r="J1" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="9" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2"/>
       <c r="D2"/>
       <c r="H2" s="10"/>
       <c r="J2" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="9"/>
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
       <c r="H3" s="10"/>
       <c r="J3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="K4" s="5"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K5" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1388,11 +2330,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E9C5AA-9540-45DB-BCC0-5EA98DDA6B0B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,30 +2361,16 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1452,11 +2380,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFF3D0A7-17A8-4B35-89BF-E7F3088D1597}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D38" sqref="D38:D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1475,7 +2403,7 @@
         <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>14</v>
@@ -1483,92 +2411,567 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B2" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B3" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B4" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B5" t="str">
         <f>"1"</f>
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" t="str">
         <f>"2"</f>
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" t="s">
         <v>82</v>
-      </c>
-      <c r="D6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B7" t="str">
         <f>"3"</f>
         <v>3</v>
       </c>
       <c r="C7" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" t="s">
         <v>83</v>
       </c>
-      <c r="D7" t="s">
-        <v>85</v>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B8" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>183</v>
+      </c>
+      <c r="D8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B9" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>187</v>
+      </c>
+      <c r="D10" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+      <c r="D11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B12" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D12" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" t="str">
+        <f>"4"</f>
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>193</v>
+      </c>
+      <c r="D13" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" t="str">
+        <f>"5"</f>
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>185</v>
+      </c>
+      <c r="D14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="str">
+        <f>"6"</f>
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>195</v>
+      </c>
+      <c r="D15" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B16" t="str">
+        <f>"88"</f>
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" t="str">
+        <f>"99"</f>
+        <v>99</v>
+      </c>
+      <c r="C17" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>174</v>
+      </c>
+      <c r="B18" t="s">
+        <v>201</v>
+      </c>
+      <c r="C18" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>174</v>
+      </c>
+      <c r="B19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C19" t="s">
+        <v>204</v>
+      </c>
+      <c r="D19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>174</v>
+      </c>
+      <c r="B20" t="s">
+        <v>206</v>
+      </c>
+      <c r="C20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" t="s">
+        <v>210</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>174</v>
+      </c>
+      <c r="B22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D22" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>177</v>
+      </c>
+      <c r="B23" t="s">
+        <v>214</v>
+      </c>
+      <c r="C23" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>177</v>
+      </c>
+      <c r="B24" t="s">
+        <v>217</v>
+      </c>
+      <c r="C24" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B25" t="s">
+        <v>220</v>
+      </c>
+      <c r="C25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>177</v>
+      </c>
+      <c r="B26" t="s">
+        <v>223</v>
+      </c>
+      <c r="C26" t="s">
+        <v>224</v>
+      </c>
+      <c r="D26" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>177</v>
+      </c>
+      <c r="B27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C27" t="s">
+        <v>227</v>
+      </c>
+      <c r="D27" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>177</v>
+      </c>
+      <c r="B28" t="s">
+        <v>229</v>
+      </c>
+      <c r="C28" t="s">
+        <v>230</v>
+      </c>
+      <c r="D28" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>177</v>
+      </c>
+      <c r="B29" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" t="s">
+        <v>233</v>
+      </c>
+      <c r="D29" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>177</v>
+      </c>
+      <c r="B30" t="s">
+        <v>235</v>
+      </c>
+      <c r="C30" t="s">
+        <v>236</v>
+      </c>
+      <c r="D30" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>238</v>
+      </c>
+      <c r="C31" t="s">
+        <v>239</v>
+      </c>
+      <c r="D31" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>148</v>
+      </c>
+      <c r="B32" t="s">
+        <v>241</v>
+      </c>
+      <c r="C32" t="s">
+        <v>242</v>
+      </c>
+      <c r="D32" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>244</v>
+      </c>
+      <c r="C33" t="s">
+        <v>245</v>
+      </c>
+      <c r="D33" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>148</v>
+      </c>
+      <c r="B34" t="s">
+        <v>247</v>
+      </c>
+      <c r="C34" t="s">
+        <v>248</v>
+      </c>
+      <c r="D34" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>148</v>
+      </c>
+      <c r="B35" t="s">
+        <v>250</v>
+      </c>
+      <c r="C35" t="s">
+        <v>251</v>
+      </c>
+      <c r="D35" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>148</v>
+      </c>
+      <c r="B36" t="s">
+        <v>253</v>
+      </c>
+      <c r="C36" t="s">
+        <v>254</v>
+      </c>
+      <c r="D36" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>148</v>
+      </c>
+      <c r="B37" t="s">
+        <v>256</v>
+      </c>
+      <c r="C37" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B38" t="str">
+        <f>"1"</f>
+        <v>1</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B39" t="str">
+        <f>"2"</f>
+        <v>2</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="B40" t="str">
+        <f>"3"</f>
+        <v>3</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -1579,11 +2982,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCD3AC6-97A9-4343-AD51-53B42E3E4B29}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:C51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,10 +3009,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1617,7 +3020,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -1628,10 +3031,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="b">
         <v>0</v>
@@ -1639,10 +3042,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C5" t="b">
         <v>0</v>
@@ -1650,7 +3053,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6" t="s">
         <v>25</v>
@@ -1661,7 +3064,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
@@ -1672,7 +3075,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
         <v>25</v>
@@ -1683,7 +3086,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
         <v>25</v>
@@ -1694,32 +3097,32 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C12" t="b">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="C13" t="b">
         <v>0</v>
@@ -1727,10 +3130,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="C14" t="b">
         <v>0</v>
@@ -1740,30 +3143,30 @@
       <c r="A15" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>129</v>
+      <c r="B15" t="s">
+        <v>72</v>
       </c>
       <c r="C15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>112</v>
-      </c>
-      <c r="B17" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" t="b">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>114</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>115</v>
+        <v>108</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C18" t="b">
         <v>0</v>
@@ -1771,10 +3174,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>116</v>
-      </c>
-      <c r="B19" s="11" t="s">
-        <v>113</v>
+        <v>110</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="C19" t="b">
         <v>0</v>
@@ -1782,10 +3185,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C20" t="b">
         <v>0</v>
@@ -1793,10 +3196,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>118</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>115</v>
+        <v>113</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C21" t="b">
         <v>0</v>
@@ -1804,10 +3207,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>119</v>
-      </c>
-      <c r="B22" s="11" t="s">
-        <v>113</v>
+        <v>114</v>
+      </c>
+      <c r="B22" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="C22" t="b">
         <v>0</v>
@@ -1815,10 +3218,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C23" t="b">
         <v>0</v>
@@ -1826,10 +3229,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>134</v>
-      </c>
-      <c r="B24" s="14" t="s">
-        <v>115</v>
+        <v>128</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C24" t="b">
         <v>0</v>
@@ -1837,10 +3240,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>133</v>
-      </c>
-      <c r="B25" s="11" t="s">
-        <v>113</v>
+        <v>130</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="C25" t="b">
         <v>0</v>
@@ -1848,10 +3251,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C26" t="b">
         <v>0</v>
@@ -1859,10 +3262,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>115</v>
+        <v>116</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>109</v>
       </c>
       <c r="C27" t="b">
         <v>0</v>
@@ -1870,10 +3273,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="11" t="s">
-        <v>113</v>
+        <v>117</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="C28" t="b">
         <v>0</v>
@@ -1881,40 +3284,238 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B30" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>123</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B33" t="s">
         <v>124</v>
       </c>
-      <c r="C29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="B30" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="C30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>127</v>
-      </c>
-      <c r="B32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" t="b">
+      <c r="C33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>178</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>149</v>
+      </c>
+      <c r="B36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C36" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>168</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+      <c r="C39" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>167</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="C40" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>146</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B45" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>181</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>175</v>
+      </c>
+      <c r="B47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C48" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>170</v>
+      </c>
+      <c r="B49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>172</v>
+      </c>
+      <c r="B50" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>154</v>
+      </c>
+      <c r="B51" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
-    <sortCondition ref="A2"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:C51">
+    <sortCondition ref="A35"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>